<commit_message>
Adding contact details class
</commit_message>
<xml_diff>
--- a/TestData/TestData001 - Copy.xlsx
+++ b/TestData/TestData001 - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Java\workspace-2\mavan.HRm\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0E2D7B-3FF5-46E8-BD88-B038C3CDCC5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C35D8D1-68D6-4869-BABD-EA8AA8C77AD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
   <si>
     <t>User Name</t>
   </si>
@@ -72,6 +72,54 @@
   </si>
   <si>
     <t>12345678</t>
+  </si>
+  <si>
+    <t>OtherId</t>
+  </si>
+  <si>
+    <t>DriverLicenseNo.</t>
+  </si>
+  <si>
+    <t>SNNnumber</t>
+  </si>
+  <si>
+    <t>SINnumber</t>
+  </si>
+  <si>
+    <t>NickName</t>
+  </si>
+  <si>
+    <t>Militreyservice</t>
+  </si>
+  <si>
+    <t>1d0123</t>
+  </si>
+  <si>
+    <t>dl12345</t>
+  </si>
+  <si>
+    <t>Nick</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>5678</t>
+  </si>
+  <si>
+    <t>customerName</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>DriverLicenseDate</t>
+  </si>
+  <si>
+    <t>01/01/2000</t>
   </si>
 </sst>
 </file>
@@ -116,11 +164,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -402,28 +451,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -508,10 +566,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3BD98BC-709C-48B7-BDFE-83E7A0840DCB}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,9 +581,16 @@
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -547,8 +612,29 @@
       <c r="G1" t="s">
         <v>8</v>
       </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -569,6 +655,27 @@
       </c>
       <c r="G2" s="3" t="s">
         <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>